<commit_message>
1. Show user full name rather than login name for all kinds of data.
2. Validate region/department required input
</commit_message>
<xml_diff>
--- a/management/src/main/resources/Agency_Recruits_template.xlsx
+++ b/management/src/main/resources/Agency_Recruits_template.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="3915"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -83,9 +84,6 @@
     <t>${record.province}</t>
   </si>
   <si>
-    <t>${record.salesPerson}</t>
-  </si>
-  <si>
     <t>${record.product}</t>
   </si>
   <si>
@@ -114,6 +112,9 @@
   </si>
   <si>
     <t>${record.level}</t>
+  </si>
+  <si>
+    <t>${record.salesPersonFullName}</t>
   </si>
 </sst>
 </file>
@@ -492,40 +493,42 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="18.5703125" customWidth="1"/>
+    <col min="1" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="7" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -534,16 +537,16 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix export not contains products bug
</commit_message>
<xml_diff>
--- a/management/src/main/resources/Agency_Recruits_template.xlsx
+++ b/management/src/main/resources/Agency_Recruits_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="3915"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="3660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,9 +84,6 @@
     <t>${record.province}</t>
   </si>
   <si>
-    <t>${record.product}</t>
-  </si>
-  <si>
     <t>${record.date}</t>
   </si>
   <si>
@@ -115,6 +112,9 @@
   </si>
   <si>
     <t>${record.salesPersonFullName}</t>
+  </si>
+  <si>
+    <t>${record.productNamesString}</t>
   </si>
 </sst>
 </file>
@@ -493,7 +493,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,30 +505,30 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -537,16 +537,16 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>